<commit_message>
Add .in file to Week3Heap
</commit_message>
<xml_diff>
--- a/Week7/7 Runtime copy.xlsx
+++ b/Week7/7 Runtime copy.xlsx
@@ -1,26 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Desktop\MyWork\2022-1 work\Data Structure\DataStructureWorkspace\week 7\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/richard/Desktop/DSA/Week7/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5383CC3-4A72-42F8-8A94-54509C8D2982}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D0E0DA1-A74A-E244-9FEE-EE2225F8A594}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{CEB7F8C8-D50F-43F1-99EC-D054581DC40D}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{CEB7F8C8-D50F-43F1-99EC-D054581DC40D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$D$2</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$D$3:$D$6</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Sheet1!$E$2</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Sheet1!$E$3:$E$6</definedName>
-  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -99,7 +93,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -107,13 +101,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -216,7 +203,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="en-US"/>
+                <a:endParaRPr lang="en-MM"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="t"/>
@@ -254,16 +241,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.140625</c:v>
+                  <c:v>0.13803699999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.4375</c:v>
+                  <c:v>0.56625199999999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.703125</c:v>
+                  <c:v>2.2057000000000002</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.78125</c:v>
+                  <c:v>8.7157429999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -340,7 +327,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="en-US"/>
+                <a:endParaRPr lang="en-MM"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="t"/>
@@ -378,16 +365,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>7.2649999999999998E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.5625E-2</c:v>
+                  <c:v>1.6661999999999899E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.5625E-2</c:v>
+                  <c:v>3.3607999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.125E-2</c:v>
+                  <c:v>6.7782999999999996E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -453,7 +440,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-MM"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="499662943"/>
@@ -512,7 +499,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-MM"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="499649631"/>
@@ -554,7 +541,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="en-MM"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -591,7 +578,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="en-MM"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1498,112 +1485,110 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EB4CC37-DC1B-46C6-B9D8-0B13F3530076}">
   <dimension ref="B1:J49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="T10" sqref="T10"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="125" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="W6" sqref="W6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="12.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.77734375" style="1"/>
-    <col min="4" max="4" width="12.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.44140625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="13.44140625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="12.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.83203125" style="1"/>
+    <col min="4" max="4" width="12.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="13.5" style="1" customWidth="1"/>
     <col min="7" max="7" width="12.33203125" style="1" customWidth="1"/>
     <col min="8" max="8" width="13.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.88671875" style="3"/>
-    <col min="10" max="10" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.83203125" style="1"/>
+    <col min="10" max="10" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="D1" s="4" t="s">
+    <row r="1" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="D1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="4"/>
-      <c r="G1" s="4" t="s">
+      <c r="E1" s="2"/>
+      <c r="G1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="4"/>
+      <c r="H1" s="2"/>
     </row>
-    <row r="2" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="5"/>
+      <c r="F2"/>
       <c r="G2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="H2" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="5"/>
-      <c r="J2" s="3"/>
+      <c r="I2"/>
+      <c r="J2" s="1"/>
     </row>
-    <row r="3" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C3" s="1">
         <v>1000</v>
       </c>
-      <c r="D3" s="3">
-        <v>0.140625</v>
-      </c>
-      <c r="E3" s="3">
-        <v>0</v>
-      </c>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3">
+      <c r="D3" s="1">
+        <v>0.13803699999999999</v>
+      </c>
+      <c r="E3" s="1">
+        <v>7.2649999999999998E-3</v>
+      </c>
+      <c r="H3" s="1">
         <v>512</v>
       </c>
     </row>
-    <row r="4" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C4" s="1">
         <v>2000</v>
       </c>
-      <c r="D4" s="3">
-        <v>0.4375</v>
-      </c>
-      <c r="E4" s="3">
-        <v>1.5625E-2</v>
-      </c>
-      <c r="H4" s="3">
+      <c r="D4" s="1">
+        <v>0.56625199999999998</v>
+      </c>
+      <c r="E4" s="1">
+        <v>1.6661999999999899E-2</v>
+      </c>
+      <c r="H4" s="1">
         <v>1003</v>
       </c>
     </row>
-    <row r="5" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C5" s="1">
         <v>4000</v>
       </c>
-      <c r="D5" s="3">
-        <v>1.703125</v>
-      </c>
-      <c r="E5" s="3">
-        <v>1.5625E-2</v>
-      </c>
-      <c r="H5" s="3">
+      <c r="D5" s="1">
+        <v>2.2057000000000002</v>
+      </c>
+      <c r="E5" s="1">
+        <v>3.3607999999999999E-2</v>
+      </c>
+      <c r="H5" s="1">
         <v>2050</v>
       </c>
     </row>
-    <row r="6" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C6" s="1">
         <v>8000</v>
       </c>
-      <c r="D6" s="3">
-        <v>6.78125</v>
-      </c>
-      <c r="E6" s="3">
-        <v>3.125E-2</v>
-      </c>
-      <c r="H6" s="3">
+      <c r="D6" s="1">
+        <v>8.7157429999999998</v>
+      </c>
+      <c r="E6" s="1">
+        <v>6.7782999999999996E-2</v>
+      </c>
+      <c r="H6" s="1">
         <v>4028</v>
       </c>
     </row>
-    <row r="8" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C8" s="1" t="s">
         <v>1</v>
       </c>
@@ -1614,58 +1599,40 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="E10" s="2"/>
-    </row>
-    <row r="42" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B42" s="4"/>
-      <c r="C42" s="4"/>
-      <c r="D42" s="4"/>
-      <c r="E42" s="2"/>
+    <row r="42" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B42" s="2"/>
+      <c r="C42" s="2"/>
+      <c r="D42" s="2"/>
       <c r="G42"/>
     </row>
-    <row r="43" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B43" s="4"/>
-      <c r="C43" s="4"/>
-      <c r="D43" s="4"/>
-      <c r="E43" s="2"/>
-      <c r="G43" s="2"/>
+    <row r="43" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B43" s="2"/>
+      <c r="C43" s="2"/>
+      <c r="D43" s="2"/>
     </row>
-    <row r="44" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B44"/>
       <c r="D44"/>
-      <c r="E44" s="2"/>
-      <c r="G44" s="2"/>
     </row>
-    <row r="45" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B45"/>
       <c r="D45"/>
-      <c r="E45" s="2"/>
-      <c r="G45" s="2"/>
     </row>
-    <row r="46" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B46"/>
       <c r="D46"/>
-      <c r="E46" s="2"/>
-      <c r="G46" s="2"/>
     </row>
-    <row r="47" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B47"/>
       <c r="D47"/>
-      <c r="E47" s="2"/>
-      <c r="G47" s="2"/>
     </row>
-    <row r="48" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B48"/>
       <c r="D48"/>
-      <c r="E48" s="2"/>
-      <c r="G48" s="2"/>
     </row>
-    <row r="49" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B49"/>
       <c r="D49"/>
-      <c r="E49" s="2"/>
-      <c r="G49" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>